<commit_message>
renaming counts file to supdataset1
</commit_message>
<xml_diff>
--- a/Data_Files/SRA_metadata_MVI_062623.xlsx
+++ b/Data_Files/SRA_metadata_MVI_062623.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariaingersoll/Desktop/BU_Research/Davies-Gilmore/Aip_FS_2022/Aiptasia_Fed_Starved/Data_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91CD42C1-7AED-734F-9A4E-03CB0FBEE673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA739A60-EB8A-FB40-919C-59F67EF48038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1300" yWindow="880" windowWidth="25580" windowHeight="13400" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1882,6 +1882,14 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="62"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="62" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1894,22 +1902,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="77">
@@ -2443,52 +2443,52 @@
       </c>
     </row>
     <row r="3" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="41" t="s">
         <v>197</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
     </row>
     <row r="4" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="41" t="s">
         <v>198</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
     </row>
     <row r="5" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="42" t="s">
         <v>199</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
     </row>
     <row r="6" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="42"/>
     </row>
     <row r="7" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="21" t="s">
@@ -2548,15 +2548,15 @@
       </c>
     </row>
     <row r="17" spans="2:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
     </row>
     <row r="18" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="19" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2588,27 +2588,27 @@
       <c r="B37" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="C37" s="35" t="s">
+      <c r="C37" s="39" t="s">
         <v>201</v>
       </c>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="36"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="40"/>
+      <c r="G37" s="40"/>
+      <c r="H37" s="40"/>
     </row>
     <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="C38" s="35" t="s">
+      <c r="C38" s="39" t="s">
         <v>202</v>
       </c>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="40"/>
+      <c r="F38" s="40"/>
+      <c r="G38" s="40"/>
+      <c r="H38" s="40"/>
     </row>
     <row r="41" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B41" s="21" t="s">
@@ -2679,9 +2679,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2758,13 +2758,13 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="35" t="s">
         <v>261</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="36" t="s">
         <v>281</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="37" t="s">
         <v>301</v>
       </c>
       <c r="D2" s="11" t="s">
@@ -2785,7 +2785,7 @@
       <c r="I2" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="J2" s="47" t="s">
+      <c r="J2" s="38" t="s">
         <v>324</v>
       </c>
       <c r="K2" s="11" t="s">
@@ -2796,13 +2796,13 @@
       </c>
     </row>
     <row r="3" spans="1:17" ht="340" x14ac:dyDescent="0.2">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="35" t="s">
         <v>262</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="36" t="s">
         <v>282</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="37" t="s">
         <v>301</v>
       </c>
       <c r="D3" s="11" t="s">
@@ -2823,7 +2823,7 @@
       <c r="I3" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="J3" s="47" t="s">
+      <c r="J3" s="38" t="s">
         <v>324</v>
       </c>
       <c r="K3" s="11" t="s">
@@ -2834,13 +2834,13 @@
       </c>
     </row>
     <row r="4" spans="1:17" ht="340" x14ac:dyDescent="0.2">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="35" t="s">
         <v>263</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="36" t="s">
         <v>283</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="37" t="s">
         <v>301</v>
       </c>
       <c r="D4" s="11" t="s">
@@ -2861,7 +2861,7 @@
       <c r="I4" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="J4" s="47" t="s">
+      <c r="J4" s="38" t="s">
         <v>324</v>
       </c>
       <c r="K4" s="11" t="s">
@@ -2872,13 +2872,13 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="340" x14ac:dyDescent="0.2">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="35" t="s">
         <v>264</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="36" t="s">
         <v>284</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="37" t="s">
         <v>301</v>
       </c>
       <c r="D5" s="11" t="s">
@@ -2899,7 +2899,7 @@
       <c r="I5" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="J5" s="47" t="s">
+      <c r="J5" s="38" t="s">
         <v>324</v>
       </c>
       <c r="K5" s="11" t="s">
@@ -2910,13 +2910,13 @@
       </c>
     </row>
     <row r="6" spans="1:17" ht="340" x14ac:dyDescent="0.2">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="35" t="s">
         <v>265</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="36" t="s">
         <v>285</v>
       </c>
-      <c r="C6" s="46" t="s">
+      <c r="C6" s="37" t="s">
         <v>301</v>
       </c>
       <c r="D6" s="11" t="s">
@@ -2937,7 +2937,7 @@
       <c r="I6" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="J6" s="47" t="s">
+      <c r="J6" s="38" t="s">
         <v>324</v>
       </c>
       <c r="K6" s="11" t="s">
@@ -2948,13 +2948,13 @@
       </c>
     </row>
     <row r="7" spans="1:17" ht="340" x14ac:dyDescent="0.2">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="35" t="s">
         <v>266</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="36" t="s">
         <v>286</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="37" t="s">
         <v>301</v>
       </c>
       <c r="D7" s="11" t="s">
@@ -2975,7 +2975,7 @@
       <c r="I7" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="J7" s="47" t="s">
+      <c r="J7" s="38" t="s">
         <v>324</v>
       </c>
       <c r="K7" s="11" t="s">
@@ -2986,13 +2986,13 @@
       </c>
     </row>
     <row r="8" spans="1:17" ht="340" x14ac:dyDescent="0.2">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="35" t="s">
         <v>267</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="36" t="s">
         <v>287</v>
       </c>
-      <c r="C8" s="46" t="s">
+      <c r="C8" s="37" t="s">
         <v>301</v>
       </c>
       <c r="D8" s="11" t="s">
@@ -3013,7 +3013,7 @@
       <c r="I8" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="J8" s="47" t="s">
+      <c r="J8" s="38" t="s">
         <v>324</v>
       </c>
       <c r="K8" s="11" t="s">
@@ -3024,13 +3024,13 @@
       </c>
     </row>
     <row r="9" spans="1:17" ht="340" x14ac:dyDescent="0.2">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="35" t="s">
         <v>268</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="36" t="s">
         <v>288</v>
       </c>
-      <c r="C9" s="46" t="s">
+      <c r="C9" s="37" t="s">
         <v>301</v>
       </c>
       <c r="D9" s="11" t="s">
@@ -3051,7 +3051,7 @@
       <c r="I9" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="J9" s="47" t="s">
+      <c r="J9" s="38" t="s">
         <v>324</v>
       </c>
       <c r="K9" s="11" t="s">
@@ -3062,13 +3062,13 @@
       </c>
     </row>
     <row r="10" spans="1:17" ht="340" x14ac:dyDescent="0.2">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="35" t="s">
         <v>269</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="36" t="s">
         <v>289</v>
       </c>
-      <c r="C10" s="46" t="s">
+      <c r="C10" s="37" t="s">
         <v>301</v>
       </c>
       <c r="D10" s="11" t="s">
@@ -3089,7 +3089,7 @@
       <c r="I10" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="J10" s="47" t="s">
+      <c r="J10" s="38" t="s">
         <v>324</v>
       </c>
       <c r="K10" s="11" t="s">
@@ -3100,13 +3100,13 @@
       </c>
     </row>
     <row r="11" spans="1:17" ht="340" x14ac:dyDescent="0.2">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="35" t="s">
         <v>270</v>
       </c>
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="36" t="s">
         <v>290</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="37" t="s">
         <v>301</v>
       </c>
       <c r="D11" s="11" t="s">
@@ -3127,7 +3127,7 @@
       <c r="I11" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="J11" s="47" t="s">
+      <c r="J11" s="38" t="s">
         <v>324</v>
       </c>
       <c r="K11" s="11" t="s">
@@ -3138,13 +3138,13 @@
       </c>
     </row>
     <row r="12" spans="1:17" ht="340" x14ac:dyDescent="0.2">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="35" t="s">
         <v>271</v>
       </c>
-      <c r="B12" s="45" t="s">
+      <c r="B12" s="36" t="s">
         <v>291</v>
       </c>
-      <c r="C12" s="46" t="s">
+      <c r="C12" s="37" t="s">
         <v>301</v>
       </c>
       <c r="D12" s="11" t="s">
@@ -3165,7 +3165,7 @@
       <c r="I12" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="J12" s="47" t="s">
+      <c r="J12" s="38" t="s">
         <v>324</v>
       </c>
       <c r="K12" s="11" t="s">
@@ -3176,13 +3176,13 @@
       </c>
     </row>
     <row r="13" spans="1:17" ht="340" x14ac:dyDescent="0.2">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="35" t="s">
         <v>272</v>
       </c>
-      <c r="B13" s="45" t="s">
+      <c r="B13" s="36" t="s">
         <v>292</v>
       </c>
-      <c r="C13" s="46" t="s">
+      <c r="C13" s="37" t="s">
         <v>301</v>
       </c>
       <c r="D13" s="11" t="s">
@@ -3203,7 +3203,7 @@
       <c r="I13" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="J13" s="47" t="s">
+      <c r="J13" s="38" t="s">
         <v>324</v>
       </c>
       <c r="K13" s="11" t="s">
@@ -3214,13 +3214,13 @@
       </c>
     </row>
     <row r="14" spans="1:17" ht="340" x14ac:dyDescent="0.2">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="35" t="s">
         <v>273</v>
       </c>
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="36" t="s">
         <v>293</v>
       </c>
-      <c r="C14" s="46" t="s">
+      <c r="C14" s="37" t="s">
         <v>301</v>
       </c>
       <c r="D14" s="11" t="s">
@@ -3241,7 +3241,7 @@
       <c r="I14" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="J14" s="47" t="s">
+      <c r="J14" s="38" t="s">
         <v>324</v>
       </c>
       <c r="K14" s="11" t="s">
@@ -3252,13 +3252,13 @@
       </c>
     </row>
     <row r="15" spans="1:17" ht="340" x14ac:dyDescent="0.2">
-      <c r="A15" s="44" t="s">
+      <c r="A15" s="35" t="s">
         <v>274</v>
       </c>
-      <c r="B15" s="45" t="s">
+      <c r="B15" s="36" t="s">
         <v>294</v>
       </c>
-      <c r="C15" s="46" t="s">
+      <c r="C15" s="37" t="s">
         <v>301</v>
       </c>
       <c r="D15" s="11" t="s">
@@ -3279,7 +3279,7 @@
       <c r="I15" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="J15" s="47" t="s">
+      <c r="J15" s="38" t="s">
         <v>324</v>
       </c>
       <c r="K15" s="11" t="s">
@@ -3290,13 +3290,13 @@
       </c>
     </row>
     <row r="16" spans="1:17" ht="340" x14ac:dyDescent="0.2">
-      <c r="A16" s="44" t="s">
+      <c r="A16" s="35" t="s">
         <v>275</v>
       </c>
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="36" t="s">
         <v>295</v>
       </c>
-      <c r="C16" s="46" t="s">
+      <c r="C16" s="37" t="s">
         <v>301</v>
       </c>
       <c r="D16" s="11" t="s">
@@ -3317,7 +3317,7 @@
       <c r="I16" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="J16" s="47" t="s">
+      <c r="J16" s="38" t="s">
         <v>324</v>
       </c>
       <c r="K16" s="11" t="s">
@@ -3328,13 +3328,13 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="340" x14ac:dyDescent="0.2">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="35" t="s">
         <v>276</v>
       </c>
-      <c r="B17" s="45" t="s">
+      <c r="B17" s="36" t="s">
         <v>296</v>
       </c>
-      <c r="C17" s="46" t="s">
+      <c r="C17" s="37" t="s">
         <v>301</v>
       </c>
       <c r="D17" s="11" t="s">
@@ -3355,7 +3355,7 @@
       <c r="I17" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="J17" s="47" t="s">
+      <c r="J17" s="38" t="s">
         <v>324</v>
       </c>
       <c r="K17" s="11" t="s">
@@ -3366,13 +3366,13 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="340" x14ac:dyDescent="0.2">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="35" t="s">
         <v>277</v>
       </c>
-      <c r="B18" s="45" t="s">
+      <c r="B18" s="36" t="s">
         <v>297</v>
       </c>
-      <c r="C18" s="46" t="s">
+      <c r="C18" s="37" t="s">
         <v>301</v>
       </c>
       <c r="D18" s="11" t="s">
@@ -3393,7 +3393,7 @@
       <c r="I18" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="J18" s="47" t="s">
+      <c r="J18" s="38" t="s">
         <v>324</v>
       </c>
       <c r="K18" s="11" t="s">
@@ -3404,13 +3404,13 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="340" x14ac:dyDescent="0.2">
-      <c r="A19" s="44" t="s">
+      <c r="A19" s="35" t="s">
         <v>278</v>
       </c>
-      <c r="B19" s="45" t="s">
+      <c r="B19" s="36" t="s">
         <v>298</v>
       </c>
-      <c r="C19" s="46" t="s">
+      <c r="C19" s="37" t="s">
         <v>301</v>
       </c>
       <c r="D19" s="11" t="s">
@@ -3431,7 +3431,7 @@
       <c r="I19" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="J19" s="47" t="s">
+      <c r="J19" s="38" t="s">
         <v>324</v>
       </c>
       <c r="K19" s="11" t="s">
@@ -3442,13 +3442,13 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="340" x14ac:dyDescent="0.2">
-      <c r="A20" s="44" t="s">
+      <c r="A20" s="35" t="s">
         <v>279</v>
       </c>
-      <c r="B20" s="45" t="s">
+      <c r="B20" s="36" t="s">
         <v>299</v>
       </c>
-      <c r="C20" s="46" t="s">
+      <c r="C20" s="37" t="s">
         <v>301</v>
       </c>
       <c r="D20" s="11" t="s">
@@ -3469,7 +3469,7 @@
       <c r="I20" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="J20" s="47" t="s">
+      <c r="J20" s="38" t="s">
         <v>324</v>
       </c>
       <c r="K20" s="11" t="s">
@@ -3480,13 +3480,13 @@
       </c>
     </row>
     <row r="21" spans="1:12" ht="340" x14ac:dyDescent="0.2">
-      <c r="A21" s="44" t="s">
+      <c r="A21" s="35" t="s">
         <v>280</v>
       </c>
-      <c r="B21" s="45" t="s">
+      <c r="B21" s="36" t="s">
         <v>300</v>
       </c>
-      <c r="C21" s="46" t="s">
+      <c r="C21" s="37" t="s">
         <v>301</v>
       </c>
       <c r="D21" s="11" t="s">
@@ -3507,7 +3507,7 @@
       <c r="I21" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="J21" s="47" t="s">
+      <c r="J21" s="38" t="s">
         <v>324</v>
       </c>
       <c r="K21" s="11" t="s">
@@ -3518,7 +3518,7 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C22" s="46"/>
+      <c r="C22" s="37"/>
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
@@ -5967,15 +5967,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
     </row>
     <row r="2" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="43"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="46"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -5987,172 +5987,172 @@
       <c r="A3" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="44" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="40"/>
+      <c r="C3" s="44"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="C4" s="40"/>
+      <c r="C4" s="44"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="40"/>
+      <c r="C5" s="44"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="C6" s="40"/>
+      <c r="C6" s="44"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="44" t="s">
         <v>114</v>
       </c>
-      <c r="C7" s="40"/>
+      <c r="C7" s="44"/>
     </row>
     <row r="8" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="44" t="s">
         <v>115</v>
       </c>
-      <c r="C8" s="40"/>
+      <c r="C8" s="44"/>
     </row>
     <row r="9" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="44" t="s">
         <v>116</v>
       </c>
-      <c r="C9" s="40"/>
+      <c r="C9" s="44"/>
     </row>
     <row r="10" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="44" t="s">
         <v>117</v>
       </c>
-      <c r="C10" s="40"/>
+      <c r="C10" s="44"/>
     </row>
     <row r="11" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="44" t="s">
         <v>118</v>
       </c>
-      <c r="C11" s="40"/>
+      <c r="C11" s="44"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="C12" s="40"/>
+      <c r="C12" s="44"/>
     </row>
     <row r="13" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="44" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="40"/>
+      <c r="C13" s="44"/>
     </row>
     <row r="14" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="C14" s="40"/>
+      <c r="C14" s="44"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="C15" s="40"/>
+      <c r="C15" s="44"/>
     </row>
     <row r="16" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="C16" s="40"/>
+      <c r="C16" s="44"/>
     </row>
     <row r="17" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="44" t="s">
         <v>124</v>
       </c>
-      <c r="C17" s="40"/>
+      <c r="C17" s="44"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="C18" s="40"/>
+      <c r="C18" s="44"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="40" t="s">
+      <c r="B19" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="C19" s="40"/>
+      <c r="C19" s="44"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="44" t="s">
         <v>127</v>
       </c>
-      <c r="C20" s="40"/>
+      <c r="C20" s="44"/>
     </row>
     <row r="21" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A21" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="C21" s="40"/>
+      <c r="C21" s="44"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -6164,28 +6164,28 @@
       <c r="A22" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="C22" s="40"/>
+      <c r="C22" s="44"/>
     </row>
     <row r="23" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="C23" s="40"/>
+      <c r="C23" s="44"/>
     </row>
     <row r="24" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="B24" s="40" t="s">
+      <c r="B24" s="44" t="s">
         <v>131</v>
       </c>
-      <c r="C24" s="40"/>
+      <c r="C24" s="44"/>
     </row>
     <row r="25" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
@@ -6289,75 +6289,75 @@
       <c r="A37" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="B37" s="40" t="s">
+      <c r="B37" s="44" t="s">
         <v>132</v>
       </c>
-      <c r="C37" s="40"/>
+      <c r="C37" s="44"/>
     </row>
     <row r="38" spans="1:3" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="40"/>
-      <c r="C38" s="40"/>
+      <c r="B38" s="44"/>
+      <c r="C38" s="44"/>
     </row>
     <row r="39" spans="1:3" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A39" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="42"/>
-      <c r="C39" s="43"/>
+      <c r="B39" s="45"/>
+      <c r="C39" s="46"/>
     </row>
     <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="B40" s="40" t="s">
+      <c r="B40" s="44" t="s">
         <v>133</v>
       </c>
-      <c r="C40" s="40"/>
+      <c r="C40" s="44"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="B41" s="40" t="s">
+      <c r="B41" s="44" t="s">
         <v>134</v>
       </c>
-      <c r="C41" s="40"/>
+      <c r="C41" s="44"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A42" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="B42" s="40" t="s">
+      <c r="B42" s="44" t="s">
         <v>135</v>
       </c>
-      <c r="C42" s="40"/>
+      <c r="C42" s="44"/>
     </row>
     <row r="43" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="B43" s="40" t="s">
+      <c r="B43" s="44" t="s">
         <v>136</v>
       </c>
-      <c r="C43" s="40"/>
+      <c r="C43" s="44"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A44" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="B44" s="40" t="s">
+      <c r="B44" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="C44" s="40"/>
+      <c r="C44" s="44"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A45" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="B45" s="40" t="s">
+      <c r="B45" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="C45" s="40"/>
+      <c r="C45" s="44"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46" s="2" t="s">
@@ -6373,264 +6373,264 @@
       <c r="A48" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="B48" s="40" t="s">
+      <c r="B48" s="44" t="s">
         <v>139</v>
       </c>
-      <c r="C48" s="40"/>
+      <c r="C48" s="44"/>
     </row>
     <row r="49" spans="1:3" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="40"/>
-      <c r="C49" s="40"/>
+      <c r="B49" s="44"/>
+      <c r="C49" s="44"/>
     </row>
     <row r="50" spans="1:3" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A50" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B50" s="41"/>
-      <c r="C50" s="40"/>
+      <c r="B50" s="47"/>
+      <c r="C50" s="44"/>
     </row>
     <row r="51" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="B51" s="40" t="s">
+      <c r="B51" s="44" t="s">
         <v>140</v>
       </c>
-      <c r="C51" s="40"/>
+      <c r="C51" s="44"/>
     </row>
     <row r="52" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="B52" s="40" t="s">
+      <c r="B52" s="44" t="s">
         <v>141</v>
       </c>
-      <c r="C52" s="40"/>
+      <c r="C52" s="44"/>
     </row>
     <row r="53" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="B53" s="40" t="s">
+      <c r="B53" s="44" t="s">
         <v>142</v>
       </c>
-      <c r="C53" s="40"/>
+      <c r="C53" s="44"/>
     </row>
     <row r="54" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="B54" s="40" t="s">
+      <c r="B54" s="44" t="s">
         <v>143</v>
       </c>
-      <c r="C54" s="40"/>
+      <c r="C54" s="44"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A55" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="B55" s="40" t="s">
+      <c r="B55" s="44" t="s">
         <v>144</v>
       </c>
-      <c r="C55" s="40"/>
+      <c r="C55" s="44"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A56" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="B56" s="40" t="s">
+      <c r="B56" s="44" t="s">
         <v>145</v>
       </c>
-      <c r="C56" s="40"/>
+      <c r="C56" s="44"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A57" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="B57" s="40" t="s">
+      <c r="B57" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="C57" s="40"/>
+      <c r="C57" s="44"/>
     </row>
     <row r="58" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="B58" s="40" t="s">
+      <c r="B58" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="C58" s="40"/>
+      <c r="C58" s="44"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A59" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="B59" s="40" t="s">
+      <c r="B59" s="44" t="s">
         <v>148</v>
       </c>
-      <c r="C59" s="40"/>
+      <c r="C59" s="44"/>
     </row>
     <row r="60" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="B60" s="40" t="s">
+      <c r="B60" s="44" t="s">
         <v>149</v>
       </c>
-      <c r="C60" s="40"/>
+      <c r="C60" s="44"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A61" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="B61" s="40" t="s">
+      <c r="B61" s="44" t="s">
         <v>150</v>
       </c>
-      <c r="C61" s="40"/>
+      <c r="C61" s="44"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A62" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="B62" s="40" t="s">
+      <c r="B62" s="44" t="s">
         <v>151</v>
       </c>
-      <c r="C62" s="40"/>
+      <c r="C62" s="44"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A63" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="B63" s="40" t="s">
+      <c r="B63" s="44" t="s">
         <v>152</v>
       </c>
-      <c r="C63" s="40"/>
+      <c r="C63" s="44"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A64" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="B64" s="40" t="s">
+      <c r="B64" s="44" t="s">
         <v>153</v>
       </c>
-      <c r="C64" s="40"/>
+      <c r="C64" s="44"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A65" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="B65" s="40" t="s">
+      <c r="B65" s="44" t="s">
         <v>154</v>
       </c>
-      <c r="C65" s="40"/>
+      <c r="C65" s="44"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A66" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="B66" s="40" t="s">
+      <c r="B66" s="44" t="s">
         <v>155</v>
       </c>
-      <c r="C66" s="40"/>
+      <c r="C66" s="44"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A67" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="B67" s="40" t="s">
+      <c r="B67" s="44" t="s">
         <v>156</v>
       </c>
-      <c r="C67" s="40"/>
+      <c r="C67" s="44"/>
     </row>
     <row r="68" spans="1:3" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="B68" s="40" t="s">
+      <c r="B68" s="44" t="s">
         <v>157</v>
       </c>
-      <c r="C68" s="40"/>
+      <c r="C68" s="44"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A69" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="B69" s="40" t="s">
+      <c r="B69" s="44" t="s">
         <v>158</v>
       </c>
-      <c r="C69" s="40"/>
+      <c r="C69" s="44"/>
     </row>
     <row r="70" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="B70" s="40" t="s">
+      <c r="B70" s="44" t="s">
         <v>159</v>
       </c>
-      <c r="C70" s="40"/>
+      <c r="C70" s="44"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A71" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="B71" s="40" t="s">
+      <c r="B71" s="44" t="s">
         <v>160</v>
       </c>
-      <c r="C71" s="40"/>
+      <c r="C71" s="44"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A72" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="B72" s="40" t="s">
+      <c r="B72" s="44" t="s">
         <v>161</v>
       </c>
-      <c r="C72" s="40"/>
+      <c r="C72" s="44"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A73" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="B73" s="40" t="s">
+      <c r="B73" s="44" t="s">
         <v>162</v>
       </c>
-      <c r="C73" s="40"/>
+      <c r="C73" s="44"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A74" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="B74" s="40" t="s">
+      <c r="B74" s="44" t="s">
         <v>163</v>
       </c>
-      <c r="C74" s="40"/>
+      <c r="C74" s="44"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A75" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="B75" s="40" t="s">
+      <c r="B75" s="44" t="s">
         <v>164</v>
       </c>
-      <c r="C75" s="40"/>
+      <c r="C75" s="44"/>
     </row>
     <row r="76" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="B76" s="40" t="s">
+      <c r="B76" s="44" t="s">
         <v>165</v>
       </c>
-      <c r="C76" s="40"/>
+      <c r="C76" s="44"/>
     </row>
     <row r="77" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B77" s="40" t="s">
+      <c r="B77" s="44" t="s">
         <v>166</v>
       </c>
-      <c r="C77" s="40"/>
+      <c r="C77" s="44"/>
     </row>
     <row r="78" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="2" t="s">
@@ -6983,25 +6983,38 @@
     <sortCondition ref="J87"/>
   </sortState>
   <mergeCells count="63">
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
@@ -7014,38 +7027,25 @@
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>